<commit_message>
added gregorian date to spreadsheet
</commit_message>
<xml_diff>
--- a/LightTime_toVenus.xlsx
+++ b/LightTime_toVenus.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Julian Date</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>One-way light seconds</t>
+  </si>
+  <si>
+    <t>Gregorian Date</t>
+  </si>
+  <si>
+    <t>Excel epoch</t>
   </si>
 </sst>
 </file>
@@ -74,7 +80,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -82,6 +88,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D142"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,9 +380,11 @@
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -384,8 +393,14 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -396,8 +411,12 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2"/>
+      <c r="F2">
+        <v>2415018.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2441413.5</v>
       </c>
@@ -410,8 +429,12 @@
       <c r="D3">
         <v>5.6963516016406697</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="3">
+        <f>A3-$F$2</f>
+        <v>26395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2441414.5</v>
       </c>
@@ -424,8 +447,12 @@
       <c r="D4">
         <v>11.3910389414224</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="3">
+        <f t="shared" ref="E4:E67" si="0">A4-$F$2</f>
+        <v>26396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2441415.5</v>
       </c>
@@ -438,8 +465,12 @@
       <c r="D5">
         <v>17.082399748168701</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>26397</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2441416.5</v>
       </c>
@@ -452,8 +483,12 @@
       <c r="D6">
         <v>22.7687742337787</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>26398</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2441417.5</v>
       </c>
@@ -466,8 +501,12 @@
       <c r="D7">
         <v>28.448505363082099</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>26399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2441418.5</v>
       </c>
@@ -480,8 +519,12 @@
       <c r="D8">
         <v>34.119939125280403</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>26400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2441419.5</v>
       </c>
@@ -494,8 +537,12 @@
       <c r="D9">
         <v>39.781424807395197</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>26401</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2441420.5</v>
       </c>
@@ -508,8 +555,12 @@
       <c r="D10">
         <v>45.4313152699754</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>26402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2441421.5</v>
       </c>
@@ -522,8 +573,12 @@
       <c r="D11">
         <v>51.067967225678103</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>26403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2441422.5</v>
       </c>
@@ -536,8 +591,12 @@
       <c r="D12">
         <v>56.689741520902501</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>26404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2441423.5</v>
       </c>
@@ -550,8 +609,12 @@
       <c r="D13">
         <v>62.295003421071101</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>26405</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2441424.5</v>
       </c>
@@ -564,8 +627,12 @@
       <c r="D14">
         <v>67.882122899824907</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>26406</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2441425.5</v>
       </c>
@@ -578,8 +645,12 @@
       <c r="D15">
         <v>73.449474932799902</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>26407</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2441426.5</v>
       </c>
@@ -592,8 +663,12 @@
       <c r="D16">
         <v>78.995439796243602</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>26408</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2441427.5</v>
       </c>
@@ -606,8 +681,12 @@
       <c r="D17">
         <v>84.518403371080197</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>26409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2441428.5</v>
       </c>
@@ -620,8 +699,12 @@
       <c r="D18">
         <v>90.016757452894495</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>26410</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2441429.5</v>
       </c>
@@ -634,8 +717,12 @@
       <c r="D19">
         <v>95.488900068358305</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>26411</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2441430.5</v>
       </c>
@@ -648,8 +735,12 @@
       <c r="D20">
         <v>100.933235798659</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>26412</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2441431.5</v>
       </c>
@@ -662,8 +753,12 @@
       <c r="D21">
         <v>106.348176110457</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>26413</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2441432.5</v>
       </c>
@@ -676,8 +771,12 @@
       <c r="D22">
         <v>111.732139695065</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>26414</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2441433.5</v>
       </c>
@@ -690,8 +789,12 @@
       <c r="D23">
         <v>117.08355281633401</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>26415</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2441434.5</v>
       </c>
@@ -704,8 +807,12 @@
       <c r="D24">
         <v>122.400849668018</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>26416</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2441435.5</v>
       </c>
@@ -718,8 +825,12 @@
       <c r="D25">
         <v>127.682472741184</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>26417</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2441436.5</v>
       </c>
@@ -732,8 +843,12 @@
       <c r="D26">
         <v>132.926873202416</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>26418</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2441437.5</v>
       </c>
@@ -746,8 +861,12 @@
       <c r="D27">
         <v>138.13251128366801</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>26419</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2441438.5</v>
       </c>
@@ -760,8 +879,12 @@
       <c r="D28">
         <v>143.29785668422801</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>26420</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2441439.5</v>
       </c>
@@ -774,8 +897,12 @@
       <c r="D29">
         <v>148.42138898594499</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>26421</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2441440.5</v>
       </c>
@@ -788,8 +915,12 @@
       <c r="D30">
         <v>153.50159808233599</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>26422</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2441441.5</v>
       </c>
@@ -802,8 +933,12 @@
       <c r="D31">
         <v>158.536984622456</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="3">
+        <f t="shared" si="0"/>
+        <v>26423</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2441442.5</v>
       </c>
@@ -816,8 +951,12 @@
       <c r="D32">
         <v>163.526060470602</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="3">
+        <f t="shared" si="0"/>
+        <v>26424</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2441443.5</v>
       </c>
@@ -830,8 +969,12 @@
       <c r="D33">
         <v>168.46734918263101</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="3">
+        <f t="shared" si="0"/>
+        <v>26425</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2441444.5</v>
       </c>
@@ -844,8 +987,12 @@
       <c r="D34">
         <v>173.359386499957</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="3">
+        <f t="shared" si="0"/>
+        <v>26426</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2441445.5</v>
       </c>
@@ -858,8 +1005,12 @@
       <c r="D35">
         <v>178.20072086235899</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="3">
+        <f t="shared" si="0"/>
+        <v>26427</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2441446.5</v>
       </c>
@@ -872,8 +1023,12 @@
       <c r="D36">
         <v>182.98991394050401</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="3">
+        <f t="shared" si="0"/>
+        <v>26428</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2441447.5</v>
       </c>
@@ -886,8 +1041,12 @@
       <c r="D37">
         <v>187.72554118949299</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="3">
+        <f t="shared" si="0"/>
+        <v>26429</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2441448.5</v>
       </c>
@@ -900,8 +1059,12 @@
       <c r="D38">
         <v>192.40619242458899</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="3">
+        <f t="shared" si="0"/>
+        <v>26430</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2441449.5</v>
       </c>
@@ -914,8 +1077,12 @@
       <c r="D39">
         <v>197.03047242027699</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="3">
+        <f t="shared" si="0"/>
+        <v>26431</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2441450.5</v>
       </c>
@@ -928,8 +1095,12 @@
       <c r="D40">
         <v>201.597001534052</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="3">
+        <f t="shared" si="0"/>
+        <v>26432</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2441451.5</v>
       </c>
@@ -942,8 +1113,12 @@
       <c r="D41">
         <v>206.10441635634299</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="3">
+        <f t="shared" si="0"/>
+        <v>26433</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2441452.5</v>
       </c>
@@ -956,8 +1131,12 @@
       <c r="D42">
         <v>210.55137038778301</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="3">
+        <f t="shared" si="0"/>
+        <v>26434</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2441453.5</v>
       </c>
@@ -970,8 +1149,12 @@
       <c r="D43">
         <v>214.93653474553699</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="3">
+        <f t="shared" si="0"/>
+        <v>26435</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2441454.5</v>
       </c>
@@ -984,8 +1167,12 @@
       <c r="D44">
         <v>219.25859890011699</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="3">
+        <f t="shared" si="0"/>
+        <v>26436</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2441455.5</v>
       </c>
@@ -998,8 +1185,12 @@
       <c r="D45">
         <v>223.516271444305</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="3">
+        <f t="shared" si="0"/>
+        <v>26437</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2441456.5</v>
       </c>
@@ -1012,8 +1203,12 @@
       <c r="D46">
         <v>227.70828089588201</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="3">
+        <f t="shared" si="0"/>
+        <v>26438</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2441457.5</v>
       </c>
@@ -1026,8 +1221,12 @@
       <c r="D47">
         <v>231.833376535882</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="3">
+        <f t="shared" si="0"/>
+        <v>26439</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2441458.5</v>
       </c>
@@ -1040,8 +1239,12 @@
       <c r="D48">
         <v>235.89032928422</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="3">
+        <f t="shared" si="0"/>
+        <v>26440</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2441459.5</v>
       </c>
@@ -1054,8 +1257,12 @@
       <c r="D49">
         <v>239.87793261463099</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="3">
+        <f t="shared" si="0"/>
+        <v>26441</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2441460.5</v>
       </c>
@@ -1068,8 +1275,12 @@
       <c r="D50">
         <v>243.79500351074901</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="3">
+        <f t="shared" si="0"/>
+        <v>26442</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2441461.5</v>
       </c>
@@ -1082,8 +1293,12 @@
       <c r="D51">
         <v>247.64038346555901</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="3">
+        <f t="shared" si="0"/>
+        <v>26443</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2441462.5</v>
       </c>
@@ -1096,8 +1311,12 @@
       <c r="D52">
         <v>251.41293952619699</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="3">
+        <f t="shared" si="0"/>
+        <v>26444</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2441463.5</v>
       </c>
@@ -1110,8 +1329,12 @@
       <c r="D53">
         <v>255.11156538637201</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="3">
+        <f t="shared" si="0"/>
+        <v>26445</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2441464.5</v>
       </c>
@@ -1124,8 +1347,12 @@
       <c r="D54">
         <v>258.73518252871298</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="3">
+        <f t="shared" si="0"/>
+        <v>26446</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2441465.5</v>
       </c>
@@ -1138,8 +1365,12 @@
       <c r="D55">
         <v>262.28274141932098</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="3">
+        <f t="shared" si="0"/>
+        <v>26447</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2441466.5</v>
       </c>
@@ -1152,8 +1383,12 @@
       <c r="D56">
         <v>265.75322275704701</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="3">
+        <f t="shared" si="0"/>
+        <v>26448</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2441467.5</v>
       </c>
@@ -1166,8 +1401,12 @@
       <c r="D57">
         <v>269.14563878001599</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="3">
+        <f t="shared" si="0"/>
+        <v>26449</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2441468.5</v>
       </c>
@@ -1180,8 +1419,12 @@
       <c r="D58">
         <v>272.45903463189501</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="3">
+        <f t="shared" si="0"/>
+        <v>26450</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2441469.5</v>
       </c>
@@ -1194,8 +1437,12 @@
       <c r="D59">
         <v>275.69248979071602</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="3">
+        <f t="shared" si="0"/>
+        <v>26451</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2441470.5</v>
       </c>
@@ -1208,8 +1455,12 @@
       <c r="D60">
         <v>278.84511956290697</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="3">
+        <f t="shared" si="0"/>
+        <v>26452</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2441471.5</v>
       </c>
@@ -1222,8 +1473,12 @@
       <c r="D61">
         <v>281.91607664533501</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="3">
+        <f t="shared" si="0"/>
+        <v>26453</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2441472.5</v>
       </c>
@@ -1236,8 +1491,12 @@
       <c r="D62">
         <v>284.90455275829203</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="3">
+        <f t="shared" si="0"/>
+        <v>26454</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2441473.5</v>
       </c>
@@ -1250,8 +1509,12 @@
       <c r="D63">
         <v>287.809780352296</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="3">
+        <f t="shared" si="0"/>
+        <v>26455</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2441474.5</v>
       </c>
@@ -1264,8 +1527,12 @@
       <c r="D64">
         <v>290.63103439171999</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="3">
+        <f t="shared" si="0"/>
+        <v>26456</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2441475.5</v>
       </c>
@@ -1278,8 +1545,12 @@
       <c r="D65">
         <v>293.36763421821598</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="3">
+        <f t="shared" si="0"/>
+        <v>26457</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2441476.5</v>
       </c>
@@ -1292,8 +1563,12 @@
       <c r="D66">
         <v>296.01894549702399</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="3">
+        <f t="shared" si="0"/>
+        <v>26458</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2441477.5</v>
       </c>
@@ -1306,8 +1581,12 @@
       <c r="D67">
         <v>298.58438224916199</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="3">
+        <f t="shared" si="0"/>
+        <v>26459</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2441478.5</v>
       </c>
@@ -1320,8 +1599,12 @@
       <c r="D68">
         <v>301.06340897259702</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="3">
+        <f t="shared" ref="E68:E131" si="1">A68-$F$2</f>
+        <v>26460</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2441479.5</v>
       </c>
@@ -1334,8 +1617,12 @@
       <c r="D69">
         <v>303.45554285536002</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="3">
+        <f t="shared" si="1"/>
+        <v>26461</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2441480.5</v>
       </c>
@@ -1348,8 +1635,12 @@
       <c r="D70">
         <v>305.76035608364998</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="3">
+        <f t="shared" si="1"/>
+        <v>26462</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2441481.5</v>
       </c>
@@ -1362,8 +1653,12 @@
       <c r="D71">
         <v>307.97747824778202</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="3">
+        <f t="shared" si="1"/>
+        <v>26463</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2441482.5</v>
       </c>
@@ -1376,8 +1671,12 @@
       <c r="D72">
         <v>310.10659884881801</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="3">
+        <f t="shared" si="1"/>
+        <v>26464</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2441483.5</v>
       </c>
@@ -1390,8 +1689,12 @@
       <c r="D73">
         <v>312.14746990855502</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="3">
+        <f t="shared" si="1"/>
+        <v>26465</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2441484.5</v>
       </c>
@@ -1404,8 +1707,12 @@
       <c r="D74">
         <v>314.09990868538898</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="3">
+        <f t="shared" si="1"/>
+        <v>26466</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2441485.5</v>
       </c>
@@ -1418,8 +1725,12 @@
       <c r="D75">
         <v>315.963800498328</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="3">
+        <f t="shared" si="1"/>
+        <v>26467</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2441486.5</v>
       </c>
@@ -1432,8 +1743,12 @@
       <c r="D76">
         <v>317.73910166122602</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="3">
+        <f t="shared" si="1"/>
+        <v>26468</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2441487.5</v>
       </c>
@@ -1446,8 +1761,12 @@
       <c r="D77">
         <v>319.42584252892198</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="3">
+        <f t="shared" si="1"/>
+        <v>26469</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2441488.5</v>
       </c>
@@ -1460,8 +1779,12 @@
       <c r="D78">
         <v>321.02413065665797</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="3">
+        <f t="shared" si="1"/>
+        <v>26470</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2441489.5</v>
       </c>
@@ -1474,8 +1797,12 @@
       <c r="D79">
         <v>322.53415407363701</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="3">
+        <f t="shared" si="1"/>
+        <v>26471</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2441490.5</v>
       </c>
@@ -1488,8 +1815,12 @@
       <c r="D80">
         <v>323.95618467110199</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="3">
+        <f t="shared" si="1"/>
+        <v>26472</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2441491.5</v>
       </c>
@@ -1502,8 +1833,12 @@
       <c r="D81">
         <v>325.29058170468801</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="3">
+        <f t="shared" si="1"/>
+        <v>26473</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2441492.5</v>
       </c>
@@ -1516,8 +1851,12 @@
       <c r="D82">
         <v>326.53779541004599</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="3">
+        <f t="shared" si="1"/>
+        <v>26474</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2441493.5</v>
       </c>
@@ -1530,8 +1869,12 @@
       <c r="D83">
         <v>327.698370730004</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="3">
+        <f t="shared" si="1"/>
+        <v>26475</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2441494.5</v>
       </c>
@@ -1544,8 +1887,12 @@
       <c r="D84">
         <v>328.77295115046599</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="3">
+        <f t="shared" si="1"/>
+        <v>26476</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2441495.5</v>
       </c>
@@ -1558,8 +1905,12 @@
       <c r="D85">
         <v>329.76228264129998</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="3">
+        <f t="shared" si="1"/>
+        <v>26477</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2441496.5</v>
       </c>
@@ -1572,8 +1923,12 @@
       <c r="D86">
         <v>330.66721769710801</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" s="3">
+        <f t="shared" si="1"/>
+        <v>26478</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2441497.5</v>
       </c>
@@ -1586,8 +1941,12 @@
       <c r="D87">
         <v>331.48871947153401</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="3">
+        <f t="shared" si="1"/>
+        <v>26479</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2441498.5</v>
       </c>
@@ -1600,8 +1959,12 @@
       <c r="D88">
         <v>332.22786599705</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="3">
+        <f t="shared" si="1"/>
+        <v>26480</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2441499.5</v>
       </c>
@@ -1614,8 +1977,12 @@
       <c r="D89">
         <v>332.88585448051901</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="3">
+        <f t="shared" si="1"/>
+        <v>26481</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2441500.5</v>
       </c>
@@ -1628,8 +1995,12 @@
       <c r="D90">
         <v>333.46400566284501</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="3">
+        <f t="shared" si="1"/>
+        <v>26482</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2441501.5</v>
       </c>
@@ -1642,8 +2013,12 @@
       <c r="D91">
         <v>333.96376822876402</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="3">
+        <f t="shared" si="1"/>
+        <v>26483</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2441502.5</v>
       </c>
@@ -1656,8 +2031,12 @@
       <c r="D92">
         <v>334.38672325053199</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="3">
+        <f t="shared" si="1"/>
+        <v>26484</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2441503.5</v>
       </c>
@@ -1670,8 +2049,12 @@
       <c r="D93">
         <v>334.73458864647398</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="3">
+        <f t="shared" si="1"/>
+        <v>26485</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2441504.5</v>
       </c>
@@ -1684,8 +2067,12 @@
       <c r="D94">
         <v>335.00922363245098</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="3">
+        <f t="shared" si="1"/>
+        <v>26486</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2441505.5</v>
       </c>
@@ -1698,8 +2085,12 @@
       <c r="D95">
         <v>335.21263314109302</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="3">
+        <f t="shared" si="1"/>
+        <v>26487</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2441506.5</v>
       </c>
@@ -1712,8 +2103,12 @@
       <c r="D96">
         <v>335.34697218009302</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="3">
+        <f t="shared" si="1"/>
+        <v>26488</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2441507.5</v>
       </c>
@@ -1726,8 +2121,12 @@
       <c r="D97">
         <v>335.414550097004</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="3">
+        <f t="shared" si="1"/>
+        <v>26489</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2441508.5</v>
       </c>
@@ -1740,8 +2139,12 @@
       <c r="D98">
         <v>335.41783471398998</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="3">
+        <f t="shared" si="1"/>
+        <v>26490</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2441509.5</v>
       </c>
@@ -1754,8 +2157,12 @@
       <c r="D99">
         <v>335.35945629141003</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="3">
+        <f t="shared" si="1"/>
+        <v>26491</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2441510.5</v>
       </c>
@@ -1768,8 +2175,12 @@
       <c r="D100">
         <v>335.24221127444201</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="3">
+        <f t="shared" si="1"/>
+        <v>26492</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2441511.5</v>
       </c>
@@ -1782,8 +2193,12 @@
       <c r="D101">
         <v>335.06906577219598</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="3">
+        <f t="shared" si="1"/>
+        <v>26493</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2441512.5</v>
       </c>
@@ -1796,8 +2211,12 @@
       <c r="D102">
         <v>334.84315871322002</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="3">
+        <f t="shared" si="1"/>
+        <v>26494</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2441513.5</v>
       </c>
@@ -1810,8 +2229,12 @@
       <c r="D103">
         <v>334.56780461619599</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="3">
+        <f t="shared" si="1"/>
+        <v>26495</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2441514.5</v>
       </c>
@@ -1824,8 +2247,12 @@
       <c r="D104">
         <v>334.24649590902698</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="3">
+        <f t="shared" si="1"/>
+        <v>26496</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2441515.5</v>
       </c>
@@ -1838,8 +2265,12 @@
       <c r="D105">
         <v>333.88290472393601</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="3">
+        <f t="shared" si="1"/>
+        <v>26497</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2441516.5</v>
       </c>
@@ -1852,8 +2283,12 @@
       <c r="D106">
         <v>333.48088409070402</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="3">
+        <f t="shared" si="1"/>
+        <v>26498</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2441517.5</v>
       </c>
@@ -1866,8 +2301,12 @@
       <c r="D107">
         <v>333.04446844487802</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="3">
+        <f t="shared" si="1"/>
+        <v>26499</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2441518.5</v>
       </c>
@@ -1880,8 +2319,12 @@
       <c r="D108">
         <v>332.57787336263999</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="3">
+        <f t="shared" si="1"/>
+        <v>26500</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2441519.5</v>
       </c>
@@ -1894,8 +2337,12 @@
       <c r="D109">
         <v>332.08549442972998</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="3">
+        <f t="shared" si="1"/>
+        <v>26501</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2441520.5</v>
       </c>
@@ -1908,8 +2355,12 @@
       <c r="D110">
         <v>331.57190514772498</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="3">
+        <f t="shared" si="1"/>
+        <v>26502</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2441521.5</v>
       </c>
@@ -1922,8 +2373,12 @@
       <c r="D111">
         <v>331.041853778183</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="3">
+        <f t="shared" si="1"/>
+        <v>26503</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2441522.5</v>
       </c>
@@ -1936,8 +2391,12 @@
       <c r="D112">
         <v>330.50025902350399</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="3">
+        <f t="shared" si="1"/>
+        <v>26504</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2441523.5</v>
       </c>
@@ -1950,8 +2409,12 @@
       <c r="D113">
         <v>329.95220444293699</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="3">
+        <f t="shared" si="1"/>
+        <v>26505</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2441524.5</v>
       </c>
@@ -1964,8 +2427,12 @@
       <c r="D114">
         <v>329.40293150374401</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="3">
+        <f t="shared" si="1"/>
+        <v>26506</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2441525.5</v>
       </c>
@@ -1978,8 +2445,12 @@
       <c r="D115">
         <v>328.85783117111203</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="3">
+        <f t="shared" si="1"/>
+        <v>26507</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2441526.5</v>
       </c>
@@ -1992,8 +2463,12 @@
       <c r="D116">
         <v>328.32243394633798</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" s="3">
+        <f t="shared" si="1"/>
+        <v>26508</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2441527.5</v>
       </c>
@@ -2006,8 +2481,12 @@
       <c r="D117">
         <v>327.802398271627</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117" s="3">
+        <f t="shared" si="1"/>
+        <v>26509</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2441528.5</v>
       </c>
@@ -2020,8 +2499,12 @@
       <c r="D118">
         <v>327.30349723144002</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118" s="3">
+        <f t="shared" si="1"/>
+        <v>26510</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2441529.5</v>
       </c>
@@ -2034,8 +2517,12 @@
       <c r="D119">
         <v>326.83160349541799</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119" s="3">
+        <f t="shared" si="1"/>
+        <v>26511</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2441530.5</v>
       </c>
@@ -2048,8 +2535,12 @@
       <c r="D120">
         <v>326.39267246659199</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120" s="3">
+        <f t="shared" si="1"/>
+        <v>26512</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2441531.5</v>
       </c>
@@ -2062,8 +2553,12 @@
       <c r="D121">
         <v>325.99272362028103</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121" s="3">
+        <f t="shared" si="1"/>
+        <v>26513</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2441532.5</v>
       </c>
@@ -2076,8 +2571,12 @@
       <c r="D122">
         <v>325.63782004526797</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122" s="3">
+        <f t="shared" si="1"/>
+        <v>26514</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2441533.5</v>
       </c>
@@ -2090,8 +2589,12 @@
       <c r="D123">
         <v>325.33404622760298</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123" s="3">
+        <f t="shared" si="1"/>
+        <v>26515</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2441534.5</v>
       </c>
@@ -2104,8 +2607,12 @@
       <c r="D124">
         <v>325.08748415037201</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124" s="3">
+        <f t="shared" si="1"/>
+        <v>26516</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2441535.5</v>
       </c>
@@ -2118,8 +2625,12 @@
       <c r="D125">
         <v>324.90418781730301</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125" s="3">
+        <f t="shared" si="1"/>
+        <v>26517</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2441536.5</v>
       </c>
@@ -2132,8 +2643,12 @@
       <c r="D126">
         <v>324.790156346034</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126" s="3">
+        <f t="shared" si="1"/>
+        <v>26518</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2441537.5</v>
       </c>
@@ -2146,8 +2661,12 @@
       <c r="D127">
         <v>324.75130581531101</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127" s="3">
+        <f t="shared" si="1"/>
+        <v>26519</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2441538.5</v>
       </c>
@@ -2160,8 +2679,12 @@
       <c r="D128">
         <v>324.79344008928598</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" s="3">
+        <f t="shared" si="1"/>
+        <v>26520</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2441539.5</v>
       </c>
@@ -2174,8 +2697,12 @@
       <c r="D129">
         <v>324.92222088036101</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129" s="3">
+        <f t="shared" si="1"/>
+        <v>26521</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2441540.5</v>
       </c>
@@ -2188,8 +2715,12 @@
       <c r="D130">
         <v>325.14313734801198</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" s="3">
+        <f t="shared" si="1"/>
+        <v>26522</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2441541.5</v>
       </c>
@@ -2202,8 +2733,12 @@
       <c r="D131">
         <v>325.46147556332801</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" s="3">
+        <f t="shared" si="1"/>
+        <v>26523</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2441542.5</v>
       </c>
@@ -2216,8 +2751,12 @@
       <c r="D132">
         <v>325.88228819621099</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132" s="3">
+        <f t="shared" ref="E132:E142" si="2">A132-$F$2</f>
+        <v>26524</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2441543.5</v>
       </c>
@@ -2230,8 +2769,12 @@
       <c r="D133">
         <v>326.41036480333997</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" s="3">
+        <f t="shared" si="2"/>
+        <v>26525</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2441544.5</v>
       </c>
@@ -2244,8 +2787,12 @@
       <c r="D134">
         <v>327.05020310777297</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134" s="3">
+        <f t="shared" si="2"/>
+        <v>26526</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2441545.5</v>
       </c>
@@ -2258,8 +2805,12 @@
       <c r="D135">
         <v>327.80598166573299</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135" s="3">
+        <f t="shared" si="2"/>
+        <v>26527</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2441546.5</v>
       </c>
@@ -2272,8 +2823,12 @@
       <c r="D136">
         <v>328.68153431038598</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136" s="3">
+        <f t="shared" si="2"/>
+        <v>26528</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>2441547.5</v>
       </c>
@@ -2286,8 +2841,12 @@
       <c r="D137">
         <v>329.68032674705103</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137" s="3">
+        <f t="shared" si="2"/>
+        <v>26529</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2441548.5</v>
       </c>
@@ -2300,8 +2859,12 @@
       <c r="D138">
         <v>330.80543564857498</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138" s="3">
+        <f t="shared" si="2"/>
+        <v>26530</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2441549.5</v>
       </c>
@@ -2314,8 +2877,12 @@
       <c r="D139">
         <v>332.059530563789</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139" s="3">
+        <f t="shared" si="2"/>
+        <v>26531</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2441550.5</v>
       </c>
@@ -2328,8 +2895,12 @@
       <c r="D140">
         <v>333.444858907396</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140" s="3">
+        <f t="shared" si="2"/>
+        <v>26532</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2441551.5</v>
       </c>
@@ -2342,8 +2913,12 @@
       <c r="D141">
         <v>334.96323424701501</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141" s="3">
+        <f t="shared" si="2"/>
+        <v>26533</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2441552.5</v>
       </c>
@@ -2356,12 +2931,18 @@
       <c r="D142">
         <v>336.61602804462802</v>
       </c>
+      <c r="E142" s="3">
+        <f t="shared" si="2"/>
+        <v>26534</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>